<commit_message>
Material data import by excel
</commit_message>
<xml_diff>
--- a/public/uploads/sample/sample.xlsx
+++ b/public/uploads/sample/sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Mr karim</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Sabbir Ahmed</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>details</t>
   </si>
   <si>
-    <t>stock</t>
-  </si>
-  <si>
     <t>AA</t>
   </si>
   <si>
@@ -73,6 +67,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>material_name</t>
   </si>
 </sst>
 </file>
@@ -395,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -408,127 +405,108 @@
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2">
         <v>150</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2">
         <v>500</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
         <v>750</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2">
         <v>500</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>